<commit_message>
i ebal mom excel into the mouth
</commit_message>
<xml_diff>
--- a/list_user.xlsx
+++ b/list_user.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,22 +436,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>День рождение</t>
+          <t>ФИО</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>ФИО</t>
+          <t>Дата рождения</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Логин</t>
+          <t>Родители</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Пороль</t>
+          <t>Телефон</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Почта</t>
         </is>
       </c>
     </row>
@@ -461,22 +466,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18.09.2008</t>
+          <t>Медведева Мария Петровна</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Медведева Мария Петровна</t>
+          <t>18 09 2008</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10262</t>
+          <t>Медведева Светлана Петровна</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (919) 666-14-97</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> gtnhjdbx72@mail.ru</t>
         </is>
       </c>
     </row>
@@ -486,22 +496,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>26.02.2009</t>
+          <t>Каликина Ксения Сергеевна</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Каликина Ксения Сергеевна</t>
+          <t>26 02 2009</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>82678</t>
+          <t>Каликина Алевтина Геннадьевна</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (919) 672-31-62</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>kalikina84@mail.ru</t>
         </is>
       </c>
     </row>
@@ -511,22 +526,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>02.03.2009</t>
+          <t>Николаева Анастасия Борисовна</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Николаева Анастасия Борисовна</t>
+          <t>02 03 2009</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>99081</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>12345678</t>
+          <t>Степанова Надежда Семеновна</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>89083056228</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -536,22 +554,25 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>29.01.2014</t>
+          <t>Михайлова Яна Владимировна</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Михайлова Яна Владимировна</t>
+          <t>29 01 2014</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>92351</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>12345678</t>
+          <t>Михайлова Татьяна Анатольевна</t>
+        </is>
+      </c>
+      <c r="E5" t="n">
+        <v>89083003707</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>tatiazam@mail.ru</t>
         </is>
       </c>
     </row>
@@ -561,22 +582,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>06.11.2011</t>
+          <t>Салимов Камиль Газинурович</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Салимов Камиль Газинурович</t>
+          <t>06 11 2011</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>86481</t>
+          <t>Дадюкова Елена Анатольевна</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (917) 066-59-20</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> elena.dadyukova@yandex.ru</t>
         </is>
       </c>
     </row>
@@ -586,22 +612,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17.08.2007</t>
+          <t>Прокопьева Ксения Юрьевна</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Прокопьева Ксения Юрьевна</t>
+          <t>17 08 2007</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>52848</t>
+          <t>Прокопьева Наталия Геннадьевна</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>8 987 127 10 72</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>nataliya-klubnichka@mail.ru</t>
         </is>
       </c>
     </row>
@@ -611,22 +642,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>01.07.2010</t>
+          <t>Николаев Роман Александрович</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Николаев Роман Александрович</t>
+          <t>01 07 2010</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>43780</t>
+          <t>Николаева Надежда Николаевна</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (903) 346-61-85</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Aleksandr541@inbox.ru</t>
         </is>
       </c>
     </row>
@@ -636,22 +672,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>06.04.2011</t>
+          <t>Леухин Семен Павлович</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Леухин Семен Павлович</t>
+          <t>06 04 2011</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>49242</t>
+          <t>Леухина Любовь Александровна</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (960) 302-92-02</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>gulya2182@gmail.com</t>
         </is>
       </c>
     </row>
@@ -661,22 +702,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>28.01.2021</t>
+          <t>Быстрицкий Глеб Валентинович</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Быстрицкий Глеб Валентинович</t>
+          <t>28 01 2021</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>28883</t>
+          <t>Быстрицкая Анна Константиновна</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (987) 664-56-47</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>asemenova077@gmail.com</t>
         </is>
       </c>
     </row>
@@ -686,22 +732,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>31.10.2010</t>
+          <t>Зарубин Иван Сергеевич</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>31 10 2010</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>Зарубин Иван Сергеевич</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>95614</t>
-        </is>
-      </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (908) 305-94-06</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>ingazarubina1983@gmail.com</t>
         </is>
       </c>
     </row>
@@ -711,22 +762,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>19.05.2008</t>
+          <t>Софронов Игорь Владимирович</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Софронов Игорь Владимирович</t>
+          <t>19 05 2008</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>80657</t>
+          <t>Софронова Альбина Николаевна</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>89176561722/89176510114</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -736,22 +792,25 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>29.07.2011</t>
+          <t>Краснов Кирилл Александрович</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Краснов Кирилл Александрович</t>
+          <t>29 07 2011</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>91190</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>12345678</t>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>89373827144</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -761,22 +820,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>28.11.2007</t>
+          <t>Карлинский Богдан Игоревич</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Карлинский Богдан Игоревич</t>
+          <t>28 11 2007</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>85761</t>
+          <t>Карлинская Наталья Сергеевна</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 962 599-60-00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>karlinskay@mail.ru</t>
         </is>
       </c>
     </row>
@@ -786,24 +850,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>06.07.2007</t>
+          <t>Сасаев Владимир Михайлович</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Сасаев Владимир Михайлович</t>
+          <t>06 07 2007</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>21431</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>12345678</t>
-        </is>
-      </c>
+          <t>Сасаева Ольга Александровна</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>89520299983</v>
+      </c>
+      <c r="F15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -811,22 +874,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>12.10.2006</t>
+          <t>Прокопьев Станислав Сергеевич</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Прокопьев Станислав Сергеевич</t>
+          <t>12 10 2006</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>55488</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>12345678</t>
+          <t>Прокопьева Надежда Владимировна</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>-</t>
         </is>
       </c>
     </row>
@@ -836,22 +900,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>14.04.2010</t>
+          <t>Протасов Леван Дмитриевич</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Протасов Леван Дмитриевич</t>
+          <t>14 04 2010</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>73403</t>
+          <t>Чеблуков Михаил Геннадьевич</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>7 (953) 017-94-31</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>mcheblukov@bk.ru</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
is very big changes
</commit_message>
<xml_diff>
--- a/list_user.xlsx
+++ b/list_user.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -887,7 +887,11 @@
           <t>Прокопьева Надежда Владимировна</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>-</t>

</xml_diff>

<commit_message>
change system search pupil
</commit_message>
<xml_diff>
--- a/list_user.xlsx
+++ b/list_user.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -461,7 +461,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>51144</t>
+          <t>52081</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,7 +476,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -486,7 +486,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>35705</t>
+          <t>73297</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -501,7 +501,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>73914</t>
+          <t>40338</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -526,7 +526,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -536,7 +536,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>36285</t>
+          <t>77209</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -551,7 +551,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>38727</t>
+          <t>38446</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -586,7 +586,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>31603</t>
+          <t>26754</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -601,7 +601,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>27817</t>
+          <t>57395</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -626,7 +626,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>20449</t>
+          <t>90364</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -651,7 +651,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -661,7 +661,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>70470</t>
+          <t>34967</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>81585</t>
+          <t>43969</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -701,7 +701,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>31274</t>
+          <t>40539</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -726,7 +726,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>36659</t>
+          <t>80525</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -751,7 +751,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>77442</t>
+          <t>64713</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -776,7 +776,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>62911</t>
+          <t>71808</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -811,7 +811,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>34702</t>
+          <t>51341</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>50919</t>
+          <t>84158</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -851,7 +851,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>12345678</t>
+          <t>Уже есть</t>
         </is>
       </c>
     </row>

</xml_diff>